<commit_message>
modify the data description
</commit_message>
<xml_diff>
--- a/processed_data/data_description.xlsx
+++ b/processed_data/data_description.xlsx
@@ -9,14 +9,14 @@
   <sheets>
     <sheet name="missing rates" sheetId="1" r:id="rId1"/>
     <sheet name="selected variables" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="class distribution" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39">
   <si>
     <t>Variable</t>
   </si>
@@ -84,12 +84,6 @@
     <t>Respiration rate (breaths per minute)</t>
   </si>
   <si>
-    <t>EtCO2</t>
-  </si>
-  <si>
-    <t>End tidal carbon dioxide (mm Hg)</t>
-  </si>
-  <si>
     <t>Age</t>
   </si>
   <si>
@@ -130,12 +124,19 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
       <t>For sepsis patients, </t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FFBD4147"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>SepsisLabel</t>
@@ -261,6 +262,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFBD4147"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>SepsisLabel</t>
@@ -290,10 +292,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -308,6 +310,142 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -319,154 +457,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFBD4147"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF212529"/>
-      <name val="Calibri"/>
+      <name val="Helvetica Neue"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="14.5"/>
@@ -496,103 +496,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -604,79 +670,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -720,6 +720,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -745,16 +754,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -774,21 +783,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -796,6 +790,21 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -808,162 +817,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1311,7 +1311,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="7"/>
@@ -1355,7 +1355,7 @@
         <v>1609</v>
       </c>
       <c r="D2" s="6">
-        <f>C2/(B2+C2)</f>
+        <f t="shared" ref="D2:D42" si="0">C2/(B2+C2)</f>
         <v>0.0828356672158155</v>
       </c>
       <c r="F2"/>
@@ -1373,7 +1373,7 @@
         <v>2477</v>
       </c>
       <c r="D3" s="6">
-        <f>C3/(B3+C3)</f>
+        <f t="shared" si="0"/>
         <v>0.127522652388797</v>
       </c>
       <c r="F3"/>
@@ -1391,7 +1391,7 @@
         <v>12586</v>
       </c>
       <c r="D4" s="6">
-        <f>C4/(B4+C4)</f>
+        <f t="shared" si="0"/>
         <v>0.647961285008237</v>
       </c>
       <c r="F4"/>
@@ -1409,7 +1409,7 @@
         <v>3031</v>
       </c>
       <c r="D5" s="6">
-        <f>C5/(B5+C5)</f>
+        <f t="shared" si="0"/>
         <v>0.156044069192751</v>
       </c>
       <c r="F5"/>
@@ -1427,7 +1427,7 @@
         <v>2089</v>
       </c>
       <c r="D6" s="6">
-        <f>C6/(B6+C6)</f>
+        <f t="shared" si="0"/>
         <v>0.107547364085667</v>
       </c>
       <c r="F6"/>
@@ -1445,7 +1445,7 @@
         <v>9283</v>
       </c>
       <c r="D7" s="6">
-        <f>C7/(B7+C7)</f>
+        <f t="shared" si="0"/>
         <v>0.47791392092257</v>
       </c>
       <c r="F7"/>
@@ -1463,7 +1463,7 @@
         <v>2280</v>
       </c>
       <c r="D8" s="6">
-        <f>C8/(B8+C8)</f>
+        <f t="shared" si="0"/>
         <v>0.117380560131796</v>
       </c>
       <c r="F8"/>
@@ -1475,14 +1475,14 @@
         <v>8</v>
       </c>
       <c r="B9" s="3">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3">
         <v>19424</v>
       </c>
-      <c r="C9" s="3">
-        <v>0</v>
-      </c>
       <c r="D9" s="6">
-        <f>C9/(B9+C9)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="F9"/>
       <c r="G9"/>
@@ -1499,7 +1499,7 @@
         <v>17209</v>
       </c>
       <c r="D10" s="6">
-        <f>C10/(B10+C10)</f>
+        <f t="shared" si="0"/>
         <v>0.885965815485997</v>
       </c>
       <c r="F10"/>
@@ -1517,7 +1517,7 @@
         <v>17790</v>
       </c>
       <c r="D11" s="6">
-        <f>C11/(B11+C11)</f>
+        <f t="shared" si="0"/>
         <v>0.91587726523888</v>
       </c>
       <c r="F11"/>
@@ -1535,7 +1535,7 @@
         <v>16651</v>
       </c>
       <c r="D12" s="6">
-        <f>C12/(B12+C12)</f>
+        <f t="shared" si="0"/>
         <v>0.857238467874794</v>
       </c>
       <c r="F12"/>
@@ -1553,7 +1553,7 @@
         <v>16958</v>
       </c>
       <c r="D13" s="6">
-        <f>C13/(B13+C13)</f>
+        <f t="shared" si="0"/>
         <v>0.873043657331137</v>
       </c>
       <c r="F13"/>
@@ -1571,7 +1571,7 @@
         <v>17604</v>
       </c>
       <c r="D14" s="6">
-        <f>C14/(B14+C14)</f>
+        <f t="shared" si="0"/>
         <v>0.906301482701812</v>
       </c>
       <c r="F14"/>
@@ -1589,7 +1589,7 @@
         <v>18348</v>
       </c>
       <c r="D15" s="6">
-        <f>C15/(B15+C15)</f>
+        <f t="shared" si="0"/>
         <v>0.944604612850082</v>
       </c>
       <c r="F15"/>
@@ -1607,7 +1607,7 @@
         <v>19088</v>
       </c>
       <c r="D16" s="6">
-        <f>C16/(B16+C16)</f>
+        <f t="shared" si="0"/>
         <v>0.982701812191104</v>
       </c>
       <c r="F16"/>
@@ -1625,7 +1625,7 @@
         <v>17793</v>
       </c>
       <c r="D17" s="6">
-        <f>C17/(B17+C17)</f>
+        <f t="shared" si="0"/>
         <v>0.916031713344316</v>
       </c>
     </row>
@@ -1640,7 +1640,7 @@
         <v>19093</v>
       </c>
       <c r="D18" s="6">
-        <f>C18/(B18+C18)</f>
+        <f t="shared" si="0"/>
         <v>0.982959225700165</v>
       </c>
     </row>
@@ -1655,7 +1655,7 @@
         <v>18522</v>
       </c>
       <c r="D19" s="6">
-        <f>C19/(B19+C19)</f>
+        <f t="shared" si="0"/>
         <v>0.953562602965404</v>
       </c>
     </row>
@@ -1670,7 +1670,7 @@
         <v>17757</v>
       </c>
       <c r="D20" s="6">
-        <f>C20/(B20+C20)</f>
+        <f t="shared" si="0"/>
         <v>0.914178336079077</v>
       </c>
     </row>
@@ -1685,7 +1685,7 @@
         <v>18146</v>
       </c>
       <c r="D21" s="6">
-        <f>C21/(B21+C21)</f>
+        <f t="shared" si="0"/>
         <v>0.93420510708402</v>
       </c>
     </row>
@@ -1700,7 +1700,7 @@
         <v>19384</v>
       </c>
       <c r="D22" s="6">
-        <f>C22/(B22+C22)</f>
+        <f t="shared" si="0"/>
         <v>0.997940691927512</v>
       </c>
     </row>
@@ -1715,7 +1715,7 @@
         <v>16971</v>
       </c>
       <c r="D23" s="6">
-        <f>C23/(B23+C23)</f>
+        <f t="shared" si="0"/>
         <v>0.873712932454695</v>
       </c>
     </row>
@@ -1730,7 +1730,7 @@
         <v>18647</v>
       </c>
       <c r="D24" s="6">
-        <f>C24/(B24+C24)</f>
+        <f t="shared" si="0"/>
         <v>0.959997940691928</v>
       </c>
     </row>
@@ -1745,7 +1745,7 @@
         <v>17843</v>
       </c>
       <c r="D25" s="6">
-        <f>C25/(B25+C25)</f>
+        <f t="shared" si="0"/>
         <v>0.918605848434926</v>
       </c>
     </row>
@@ -1760,7 +1760,7 @@
         <v>18476</v>
       </c>
       <c r="D26" s="6">
-        <f>C26/(B26+C26)</f>
+        <f t="shared" si="0"/>
         <v>0.951194398682043</v>
       </c>
     </row>
@@ -1775,7 +1775,7 @@
         <v>17153</v>
       </c>
       <c r="D27" s="6">
-        <f>C27/(B27+C27)</f>
+        <f t="shared" si="0"/>
         <v>0.883082784184514</v>
       </c>
     </row>
@@ -1790,7 +1790,7 @@
         <v>19182</v>
       </c>
       <c r="D28" s="6">
-        <f>C28/(B28+C28)</f>
+        <f t="shared" si="0"/>
         <v>0.98754118616145</v>
       </c>
     </row>
@@ -1805,7 +1805,7 @@
         <v>19384</v>
       </c>
       <c r="D29" s="6">
-        <f>C29/(B29+C29)</f>
+        <f t="shared" si="0"/>
         <v>0.997940691927512</v>
       </c>
     </row>
@@ -1820,7 +1820,7 @@
         <v>16965</v>
       </c>
       <c r="D30" s="6">
-        <f>C30/(B30+C30)</f>
+        <f t="shared" si="0"/>
         <v>0.873404036243822</v>
       </c>
     </row>
@@ -1835,7 +1835,7 @@
         <v>17593</v>
       </c>
       <c r="D31" s="6">
-        <f>C31/(B31+C31)</f>
+        <f t="shared" si="0"/>
         <v>0.905735172981878</v>
       </c>
     </row>
@@ -1850,7 +1850,7 @@
         <v>18477</v>
       </c>
       <c r="D32" s="6">
-        <f>C32/(B32+C32)</f>
+        <f t="shared" si="0"/>
         <v>0.951245881383855</v>
       </c>
     </row>
@@ -1865,7 +1865,7 @@
         <v>17877</v>
       </c>
       <c r="D33" s="6">
-        <f>C33/(B33+C33)</f>
+        <f t="shared" si="0"/>
         <v>0.92035626029654</v>
       </c>
     </row>
@@ -1880,7 +1880,7 @@
         <v>19224</v>
       </c>
       <c r="D34" s="6">
-        <f>C34/(B34+C34)</f>
+        <f t="shared" si="0"/>
         <v>0.989703459637562</v>
       </c>
     </row>
@@ -1895,7 +1895,7 @@
         <v>18121</v>
       </c>
       <c r="D35" s="6">
-        <f>C35/(B35+C35)</f>
+        <f t="shared" si="0"/>
         <v>0.932918039538715</v>
       </c>
     </row>
@@ -1910,7 +1910,7 @@
         <v>0</v>
       </c>
       <c r="D36" s="6">
-        <f>C36/(B36+C36)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1925,7 +1925,7 @@
         <v>0</v>
       </c>
       <c r="D37" s="6">
-        <f>C37/(B37+C37)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1940,7 +1940,7 @@
         <v>8652</v>
       </c>
       <c r="D38" s="6">
-        <f>C38/(B38+C38)</f>
+        <f t="shared" si="0"/>
         <v>0.445428336079077</v>
       </c>
     </row>
@@ -1955,7 +1955,7 @@
         <v>8652</v>
       </c>
       <c r="D39" s="6">
-        <f>C39/(B39+C39)</f>
+        <f t="shared" si="0"/>
         <v>0.445428336079077</v>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
         <v>0</v>
       </c>
       <c r="D40" s="6">
-        <f>C40/(B40+C40)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1985,7 +1985,7 @@
         <v>0</v>
       </c>
       <c r="D41" s="6">
-        <f>C41/(B41+C41)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2000,7 +2000,7 @@
         <v>0</v>
       </c>
       <c r="D42" s="6">
-        <f>C42/(B42+C42)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2016,10 +2016,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
@@ -2126,7 +2126,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" ht="14.75" spans="1:4">
+    <row r="8" spans="1:4">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2140,9 +2140,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" ht="14.75" spans="1:4">
+    <row r="9" spans="1:4">
       <c r="A9" s="3">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="B9" s="4">
         <v>0</v>
@@ -2154,9 +2154,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" ht="14.75" spans="1:4">
+    <row r="10" spans="1:4">
       <c r="A10" s="3">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B10" s="4">
         <v>0</v>
@@ -2170,10 +2170,10 @@
     </row>
     <row r="11" ht="14.75" spans="1:4">
       <c r="A11" s="3">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B11" s="4">
-        <v>0</v>
+        <v>0.445428336079077</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>26</v>
@@ -2184,7 +2184,7 @@
     </row>
     <row r="12" ht="14.75" spans="1:4">
       <c r="A12" s="3">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B12" s="4">
         <v>0.445428336079077</v>
@@ -2198,10 +2198,10 @@
     </row>
     <row r="13" ht="14.75" spans="1:4">
       <c r="A13" s="3">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B13" s="4">
-        <v>0.445428336079077</v>
+        <v>0</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>30</v>
@@ -2212,7 +2212,7 @@
     </row>
     <row r="14" ht="14.75" spans="1:4">
       <c r="A14" s="3">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B14" s="4">
         <v>0</v>
@@ -2224,9 +2224,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" ht="14.75" spans="1:4">
+    <row r="15" ht="59.75" spans="1:4">
       <c r="A15" s="3">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B15" s="4">
         <v>0</v>
@@ -2236,20 +2236,6 @@
       </c>
       <c r="D15" s="3" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="16" ht="57.75" spans="1:4">
-      <c r="A16" s="3">
-        <v>41</v>
-      </c>
-      <c r="B16" s="4">
-        <v>0</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -2264,7 +2250,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="2"/>
@@ -2274,7 +2260,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1">
         <v>0</v>
@@ -2285,7 +2271,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" s="1">
         <v>18992</v>
@@ -2296,7 +2282,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B3" s="2">
         <f>B2/(B2+C2)</f>

</xml_diff>